<commit_message>
Fix bug where the Board name is longer than excel tab name.
</commit_message>
<xml_diff>
--- a/cfd.xlsx
+++ b/cfd.xlsx
@@ -12,15 +12,15 @@
     <sheet name="CFD JAMP Team 5" sheetId="3" r:id="rId3"/>
     <sheet name="CFD JAMP Team 4" sheetId="4" r:id="rId4"/>
     <sheet name="CFD JAMP Team 1" sheetId="5" r:id="rId5"/>
-    <sheet name="CFD SKP board" sheetId="6" r:id="rId6"/>
-    <sheet name="CFD JAMP Program" sheetId="7" r:id="rId7"/>
+    <sheet name="CFD JAMP Program" sheetId="6" r:id="rId6"/>
+    <sheet name="CFD JAMP Really Super Long Boa" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="28">
   <si>
     <t>date</t>
   </si>
@@ -74,66 +74,6 @@
   </si>
   <si>
     <t>JAMP-599</t>
-  </si>
-  <si>
-    <t>Backlog</t>
-  </si>
-  <si>
-    <t>Selected for Development</t>
-  </si>
-  <si>
-    <t>SKP-14</t>
-  </si>
-  <si>
-    <t>SKP-13</t>
-  </si>
-  <si>
-    <t>SKP-15</t>
-  </si>
-  <si>
-    <t>SKP-16</t>
-  </si>
-  <si>
-    <t>SKP-12</t>
-  </si>
-  <si>
-    <t>SKP-4</t>
-  </si>
-  <si>
-    <t>SKP-11</t>
-  </si>
-  <si>
-    <t>SKP-5</t>
-  </si>
-  <si>
-    <t>SKP-6</t>
-  </si>
-  <si>
-    <t>SKP-10</t>
-  </si>
-  <si>
-    <t>SKP-9</t>
-  </si>
-  <si>
-    <t>SKP-7</t>
-  </si>
-  <si>
-    <t>SKP-8</t>
-  </si>
-  <si>
-    <t>SKP-2</t>
-  </si>
-  <si>
-    <t>SKP-1</t>
-  </si>
-  <si>
-    <t>SKP-3</t>
-  </si>
-  <si>
-    <t>10002</t>
-  </si>
-  <si>
-    <t>10003</t>
   </si>
   <si>
     <t>JAMP-1</t>
@@ -1107,13 +1047,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1130,112 +1070,100 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2">
+        <v>44272.29835648148</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>44272.29840277778</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2">
-        <v>44259.16017361111</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2">
+        <v>44272.29879629629</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>-1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2">
-        <v>44261.14975694445</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2">
+        <v>44272.681875</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C3">
-        <v>-1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2">
-        <v>44262.49767361111</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>-1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2">
-        <v>44264.47822916666</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
       <c r="C5">
         <v>-1</v>
       </c>
@@ -1243,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1254,74 +1182,65 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>44265.21920138889</v>
+        <v>44272.6883912037</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>44265.40600694445</v>
+        <v>44274.36309027778</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
-        <v>44266.7490625</v>
+        <v>44274.36346064815</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -1330,27 +1249,24 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
-        <v>44267.34697916666</v>
+        <v>44274.36349537037</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1359,172 +1275,154 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
-        <v>44267.46017361111</v>
+        <v>44274.36357638889</v>
       </c>
       <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2">
+        <v>44274.36449074074</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2">
-        <v>44267.96711805555</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
       <c r="C11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>44274.36497685185</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="2">
-        <v>44268.56711805556</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>-1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
       <c r="F12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
-        <v>44269.22961805556</v>
+        <v>44274.365</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
-        <v>44269.40809027778</v>
+        <v>44274.40775462963</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
-        <v>44269.79072916666</v>
+        <v>44274.40777777778</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1533,1034 +1431,718 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
-        <v>44270.1803125</v>
+        <v>44274.40877314815</v>
       </c>
       <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2">
+        <v>44274.40878472223</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>-1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>44274.40881944444</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2">
+        <v>44274.40883101852</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>-1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
+        <v>44274.41157407407</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2">
+        <v>44275.55016203703</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2">
-        <v>44270.3740625</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17">
-        <v>-1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17">
+      <c r="C21">
+        <v>-1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="2">
+        <v>44275.55153935185</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>4</v>
       </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="2">
-        <v>44270.49350694445</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2">
+        <v>44275.72517361111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
         <v>15</v>
       </c>
-      <c r="F18">
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>4</v>
       </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="2">
-        <v>44270.79072916666</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19">
-        <v>-1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19">
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2">
+        <v>44275.72590277778</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>-1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2">
+        <v>44275.7259375</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2">
+        <v>44277.40503472222</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="2">
+        <v>44277.40511574074</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="2">
+        <v>44278.79002314815</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>-1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2">
+        <v>44292.93833333333</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>5</v>
       </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="2">
-        <v>44271.00809027778</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="2">
-        <v>44271.01850694444</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="2">
-        <v>44271.61572916667</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22">
-        <v>4</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="2">
-        <v>44272.04072916666</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="2">
-        <v>44272.50461805556</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24">
-        <v>4</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="2">
-        <v>44272.70739583333</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="2">
-        <v>44272.79072916666</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
-        <v>-1</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26">
-        <v>4</v>
-      </c>
-      <c r="G26">
-        <v>2</v>
-      </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="2">
-        <v>44272.89628472222</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27">
-        <v>4</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27">
-        <v>2</v>
-      </c>
-      <c r="I27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="2">
-        <v>44273.01711805556</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28">
-        <v>4</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>3</v>
-      </c>
-      <c r="I28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2">
-        <v>44273.8365625</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29">
-        <v>3</v>
-      </c>
-      <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <v>3</v>
-      </c>
-      <c r="I29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
-        <v>44273.8490625</v>
+        <v>44323.52554398148</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>2</v>
-      </c>
-      <c r="I30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2">
+        <v>44323.525625</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="2">
+        <v>44323.52582175926</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="2">
+        <v>44323.5266550926</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="2">
+        <v>44330.66344907408</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <v>7</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="2">
+        <v>44330.6634837963</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35">
+        <v>7</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="2">
+        <v>44330.66351851852</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="2">
+        <v>44330.66357638889</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="2">
+        <v>44330.66359953704</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="2">
+        <v>44330.6637962963</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="2">
-        <v>44274.38447916666</v>
-      </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="2">
+        <v>44330.66383101852</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
         <v>16</v>
       </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
+      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="2">
+        <v>44334.77482638889</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41">
+        <v>-1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="2">
-        <v>44274.64628472222</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32">
-        <v>2</v>
-      </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="2">
-        <v>44274.79072916666</v>
-      </c>
-      <c r="B33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33">
-        <v>-1</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33">
-        <v>3</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="2">
-        <v>44274.79072916666</v>
-      </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34">
-        <v>-1</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34">
-        <v>4</v>
-      </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="2">
-        <v>44274.83239583333</v>
-      </c>
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-      <c r="G35">
-        <v>2</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="2">
-        <v>44275.46642361111</v>
-      </c>
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36">
-        <v>4</v>
-      </c>
-      <c r="G36">
-        <v>2</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="2">
-        <v>44275.70392361111</v>
-      </c>
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <v>3</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-      <c r="I37">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="2">
-        <v>44275.78378472223</v>
-      </c>
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38">
-        <v>4</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="2">
-        <v>44275.82267361111</v>
-      </c>
-      <c r="B39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>37</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>5</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="2">
-        <v>44276.59836805556</v>
-      </c>
-      <c r="B40" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>4</v>
-      </c>
-      <c r="H40">
-        <v>2</v>
-      </c>
-      <c r="I40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="2">
-        <v>44276.66572916666</v>
-      </c>
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
       <c r="G41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H41">
-        <v>3</v>
-      </c>
-      <c r="I41">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="2">
-        <v>44276.7490625</v>
+        <v>44334.77782407407</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
         <v>16</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>2</v>
-      </c>
-      <c r="I42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="2">
-        <v>44277.3740625</v>
-      </c>
-      <c r="B43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="H43">
-        <v>3</v>
-      </c>
-      <c r="I43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="2">
-        <v>44277.66086805556</v>
-      </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="H44">
-        <v>4</v>
-      </c>
-      <c r="I44">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="2">
-        <v>44277.77545138889</v>
-      </c>
-      <c r="B45" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>3</v>
-      </c>
-      <c r="E45" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
-        <v>3</v>
-      </c>
-      <c r="I45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="2">
-        <v>44277.79072916666</v>
-      </c>
-      <c r="B46" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46">
-        <v>-1</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>36</v>
-      </c>
-      <c r="F46">
-        <v>2</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>3</v>
-      </c>
-      <c r="I46">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="2">
-        <v>44278.5740625</v>
-      </c>
-      <c r="B47" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
-      <c r="H47">
-        <v>3</v>
-      </c>
-      <c r="I47">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="2">
-        <v>44278.68239583333</v>
-      </c>
-      <c r="B48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48">
-        <v>-1</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
-        <v>2</v>
-      </c>
-      <c r="H48">
-        <v>3</v>
-      </c>
-      <c r="I48">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="2">
-        <v>44278.75253472223</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <v>3</v>
-      </c>
-      <c r="E49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49">
-        <v>2</v>
-      </c>
-      <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49">
-        <v>2</v>
-      </c>
-      <c r="I49">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="2">
-        <v>44278.79074074074</v>
-      </c>
-      <c r="B50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50">
-        <v>-1</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50" t="s">
-        <v>36</v>
-      </c>
-      <c r="F50">
-        <v>3</v>
-      </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50">
-        <v>2</v>
-      </c>
-      <c r="I50">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2607,7 +2189,7 @@
         <v>44272.29835648148</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -2633,7 +2215,7 @@
         <v>44272.29840277778</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2659,7 +2241,7 @@
         <v>44272.29879629629</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2685,7 +2267,7 @@
         <v>44272.681875</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2711,7 +2293,7 @@
         <v>44272.6883912037</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2737,7 +2319,7 @@
         <v>44274.36309027778</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2841,7 +2423,7 @@
         <v>44274.36449074074</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2867,7 +2449,7 @@
         <v>44274.36497685185</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2893,7 +2475,7 @@
         <v>44274.365</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3075,7 +2657,7 @@
         <v>44274.41157407407</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -3101,7 +2683,7 @@
         <v>44275.55016203703</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -3127,7 +2709,7 @@
         <v>44275.55153935185</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3153,7 +2735,7 @@
         <v>44275.72517361111</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3179,7 +2761,7 @@
         <v>44275.72590277778</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -3205,7 +2787,7 @@
         <v>44275.7259375</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3231,7 +2813,7 @@
         <v>44277.40503472222</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -3257,7 +2839,7 @@
         <v>44277.40511574074</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3283,7 +2865,7 @@
         <v>44278.79002314815</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -3309,7 +2891,7 @@
         <v>44292.93833333333</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3335,7 +2917,7 @@
         <v>44323.52554398148</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3387,7 +2969,7 @@
         <v>44323.52582175926</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -3517,7 +3099,7 @@
         <v>44330.66357638889</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3621,7 +3203,7 @@
         <v>44334.77482638889</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="C41">
         <v>-1</v>

</xml_diff>